<commit_message>
Completed spread sheet with peripherals and their dependencies.
</commit_message>
<xml_diff>
--- a/Software/PeripheralDependencies.xlsx
+++ b/Software/PeripheralDependencies.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b07b1bc4cf5730b4/Documents/GitHub/Laser_Cutter/Software/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\betel\OneDrive\Documents\GitHub\Laser_Cutter\Software\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="33">
   <si>
     <t>RSTC</t>
   </si>
@@ -118,6 +118,12 @@
   </si>
   <si>
     <t>ACC</t>
+  </si>
+  <si>
+    <t>Dependencies</t>
+  </si>
+  <si>
+    <t>Peripheral</t>
   </si>
 </sst>
 </file>
@@ -153,16 +159,53 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="3">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+      <border>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <fgColor auto="1"/>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+      <border>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -472,265 +515,463 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AE32"/>
+  <dimension ref="A1:AG33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection sqref="A1:A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="31" width="7.36328125" style="1" customWidth="1"/>
-    <col min="32" max="16384" width="8.7265625" style="1"/>
+    <col min="1" max="1" width="8.7265625" style="1"/>
+    <col min="2" max="32" width="7.36328125" style="1" customWidth="1"/>
+    <col min="33" max="16384" width="8.7265625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:33" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
+      <c r="N1" s="2"/>
+      <c r="O1" s="2"/>
+      <c r="P1" s="2"/>
+      <c r="Q1" s="2"/>
+      <c r="R1" s="2"/>
+      <c r="S1" s="2"/>
+      <c r="T1" s="2"/>
+      <c r="U1" s="2"/>
+      <c r="V1" s="2"/>
+      <c r="W1" s="2"/>
+      <c r="X1" s="2"/>
+      <c r="Y1" s="2"/>
+      <c r="Z1" s="2"/>
+      <c r="AA1" s="2"/>
+      <c r="AB1" s="2"/>
+      <c r="AC1" s="2"/>
+      <c r="AD1" s="2"/>
+      <c r="AE1" s="2"/>
+      <c r="AF1" s="2"/>
+      <c r="AG1" s="2"/>
+    </row>
+    <row r="2" spans="1:33" x14ac:dyDescent="0.35">
+      <c r="A2" s="3"/>
+      <c r="C2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
+      <c r="D2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="J2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="K2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="L2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="M2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="N2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="O2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="P2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="Q2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="R2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="S2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="T2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="U2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="V2" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="W2" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="X2" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="Y2" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Z2" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="AA2" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AB2" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AC2" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AD2" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AE2" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AF2" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AG2" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="1" t="s">
+    <row r="3" spans="1:33" x14ac:dyDescent="0.35">
+      <c r="A3" s="3"/>
+      <c r="B3" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:33" x14ac:dyDescent="0.35">
+      <c r="A4" s="3"/>
+      <c r="B4" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:33" x14ac:dyDescent="0.35">
+      <c r="A5" s="3"/>
+      <c r="B5" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="1" t="s">
+    <row r="6" spans="1:33" x14ac:dyDescent="0.35">
+      <c r="A6" s="3"/>
+      <c r="B6" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="1" t="s">
+    <row r="7" spans="1:33" x14ac:dyDescent="0.35">
+      <c r="A7" s="3"/>
+      <c r="B7" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="1" t="s">
+    <row r="8" spans="1:33" x14ac:dyDescent="0.35">
+      <c r="A8" s="3"/>
+      <c r="B8" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="1" t="s">
+    <row r="9" spans="1:33" x14ac:dyDescent="0.35">
+      <c r="A9" s="3"/>
+      <c r="B9" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="1" t="s">
+    <row r="10" spans="1:33" x14ac:dyDescent="0.35">
+      <c r="A10" s="3"/>
+      <c r="B10" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="1" t="s">
+    <row r="11" spans="1:33" x14ac:dyDescent="0.35">
+      <c r="A11" s="3"/>
+      <c r="B11" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="1" t="s">
+    <row r="12" spans="1:33" x14ac:dyDescent="0.35">
+      <c r="A12" s="3"/>
+      <c r="B12" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="1" t="s">
+    <row r="13" spans="1:33" x14ac:dyDescent="0.35">
+      <c r="A13" s="3"/>
+      <c r="B13" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="1" t="s">
+    <row r="14" spans="1:33" x14ac:dyDescent="0.35">
+      <c r="A14" s="3"/>
+      <c r="B14" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="1" t="s">
+    <row r="15" spans="1:33" x14ac:dyDescent="0.35">
+      <c r="A15" s="3"/>
+      <c r="B15" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="1" t="s">
+    <row r="16" spans="1:33" x14ac:dyDescent="0.35">
+      <c r="A16" s="3"/>
+      <c r="B16" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="15" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="1" t="s">
+      <c r="Q16" s="1">
+        <v>1</v>
+      </c>
+      <c r="U16" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:33" x14ac:dyDescent="0.35">
+      <c r="A17" s="3"/>
+      <c r="B17" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="1" t="s">
+    <row r="18" spans="1:33" x14ac:dyDescent="0.35">
+      <c r="A18" s="3"/>
+      <c r="B18" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="1" t="s">
+      <c r="Q18" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:33" x14ac:dyDescent="0.35">
+      <c r="A19" s="3"/>
+      <c r="B19" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="1" t="s">
+      <c r="Q19" s="1">
+        <v>1</v>
+      </c>
+      <c r="U19" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:33" x14ac:dyDescent="0.35">
+      <c r="A20" s="3"/>
+      <c r="B20" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="1" t="s">
+    <row r="21" spans="1:33" x14ac:dyDescent="0.35">
+      <c r="A21" s="3"/>
+      <c r="B21" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="1" t="s">
+      <c r="Q21" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:33" x14ac:dyDescent="0.35">
+      <c r="A22" s="3"/>
+      <c r="B22" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="1" t="s">
+      <c r="Q22" s="1">
+        <v>1</v>
+      </c>
+      <c r="U22" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:33" x14ac:dyDescent="0.35">
+      <c r="A23" s="3"/>
+      <c r="B23" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="22" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="1" t="s">
+      <c r="Q23" s="1">
+        <v>1</v>
+      </c>
+      <c r="U23" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:33" x14ac:dyDescent="0.35">
+      <c r="A24" s="3"/>
+      <c r="B24" s="1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="23" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="1" t="s">
+      <c r="Q24" s="1">
+        <v>1</v>
+      </c>
+      <c r="U24" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:33" x14ac:dyDescent="0.35">
+      <c r="A25" s="3"/>
+      <c r="B25" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="24" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="1" t="s">
+      <c r="Q25" s="1">
+        <v>1</v>
+      </c>
+      <c r="U25" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:33" x14ac:dyDescent="0.35">
+      <c r="A26" s="3"/>
+      <c r="B26" s="1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="25" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="1" t="s">
+      <c r="Q26" s="1">
+        <v>1</v>
+      </c>
+      <c r="U26" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:33" x14ac:dyDescent="0.35">
+      <c r="A27" s="3"/>
+      <c r="B27" s="1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="26" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="1" t="s">
+      <c r="Q27" s="1">
+        <v>1</v>
+      </c>
+      <c r="U27" s="1">
+        <v>1</v>
+      </c>
+      <c r="Z27" s="1">
+        <v>1</v>
+      </c>
+      <c r="AE27" s="1">
+        <v>1</v>
+      </c>
+      <c r="AG27" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:33" x14ac:dyDescent="0.35">
+      <c r="A28" s="3"/>
+      <c r="B28" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="27" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="1" t="s">
+      <c r="Q28" s="1">
+        <v>1</v>
+      </c>
+      <c r="U28" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:33" x14ac:dyDescent="0.35">
+      <c r="A29" s="3"/>
+      <c r="B29" s="1" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="28" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="1" t="s">
+      <c r="Q29" s="1">
+        <v>1</v>
+      </c>
+      <c r="U29" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:33" x14ac:dyDescent="0.35">
+      <c r="A30" s="3"/>
+      <c r="B30" s="1" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="29" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="1" t="s">
+      <c r="Q30" s="1">
+        <v>1</v>
+      </c>
+      <c r="U30" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:33" x14ac:dyDescent="0.35">
+      <c r="A31" s="3"/>
+      <c r="B31" s="1" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="30" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="1" t="s">
+      <c r="Q31" s="1">
+        <v>1</v>
+      </c>
+      <c r="U31" s="1">
+        <v>1</v>
+      </c>
+      <c r="Z31" s="1">
+        <v>1</v>
+      </c>
+      <c r="AA31" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:33" x14ac:dyDescent="0.35">
+      <c r="A32" s="3"/>
+      <c r="B32" s="1" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="31" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="1" t="s">
+      <c r="Q32" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A33" s="3"/>
+      <c r="B33" s="1" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="32" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
+      <c r="Q33" s="1">
+        <v>1</v>
+      </c>
+      <c r="U33" s="1">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B1:AG1"/>
+    <mergeCell ref="A1:A33"/>
+  </mergeCells>
+  <conditionalFormatting sqref="C3:AF32">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AG3:AG27">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C33:AG33">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>